<commit_message>
Assembling mouse up to 06 Sept Download
Wrote mouse code to assemble all raw transcriptomes up through the 06
Sept download.
</commit_message>
<xml_diff>
--- a/data_download/transcriptome_compression_download_log.xlsx
+++ b/data_download/transcriptome_compression_download_log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Athaliana" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Download</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>$killdevil:/ms/home/s/b/sbiswas/transcriptome_compression/Athaliana/NCBI_SRA_Athaliana_successful_downloads_06Sept2015_download_compiled_23Sept2015.tgz</t>
+  </si>
+  <si>
+    <t>$killdevil:/ms/home/s/b/sbiswas/transcriptome_compression/Mmusculus/NCBI_SRA_Mmusculus_successful_downloads_19Sept2015_download_compiled_23Sept2015.tgz</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,7 +584,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -640,6 +643,9 @@
       <c r="A6" s="2">
         <v>42266</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>

</xml_diff>